<commit_message>
Update ELF II BOM regarding 74LS00 and 74HC74
</commit_message>
<xml_diff>
--- a/notes/ELF-II/AVI ELF II Final BOM.xlsx
+++ b/notes/ELF-II/AVI ELF II Final BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewwasson/Development/avi-elf-ii/notes/ELF-II/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFC7DEE-7BA0-594F-96A5-1BED7A3A0BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC558B5-0ACA-9D44-9503-FE59DA7E70FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="600" windowWidth="42520" windowHeight="22300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="600" windowWidth="42520" windowHeight="22300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DigiKey.ca" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="366">
   <si>
     <t>A1</t>
   </si>
@@ -286,9 +286,6 @@
     <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/CD4049UBE?qs=D5pVkbrsqqLvQoWdk2gTTw%3D%3D</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/texas-instruments/SN74HC00N/277209</t>
-  </si>
-  <si>
     <t>SRAM 256K-Bit (32Kx8)</t>
   </si>
   <si>
@@ -664,9 +661,6 @@
     <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/CD74HC173E?qs=j01uVdFEFjELTUIKncHz%252Bg%3D%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/SN74HC00AN?qs=6ZVwTuetbD7YqMbSpl34ug%3D%3D</t>
-  </si>
-  <si>
     <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/CD74HCT74E?qs=ZA235jQDfboKM%252BOEvlrfDA%3D%3D</t>
   </si>
   <si>
@@ -802,9 +796,6 @@
     <t>https://www.digikey.com/en/products/detail/texas-instruments/CD4049UBE/67301</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/texas-instruments/SN74HC00N/277209</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/texas-instruments/CD74HCT74E/38762</t>
   </si>
   <si>
@@ -946,9 +937,6 @@
     <t>https://www.mouser.com/ProductDetail/Texas-Instruments/CD4049UBE?qs=D5pVkbrsqqLvQoWdk2gTTw%3D%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/SN74HC00AN?qs=6ZVwTuetbD7YqMbSpl34ug%3D%3D</t>
-  </si>
-  <si>
     <t>https://www.mouser.com/ProductDetail/Texas-Instruments/CD74HCT74E?qs=ZA235jQDfboKM%252BOEvlrfDA%3D%3D</t>
   </si>
   <si>
@@ -1108,9 +1096,6 @@
     <t>Jameco Electronics: https://www.jameco.com/z/74C922-Major-Brands-IC-74C922-16-20-Key-Encoder-DIP-18-pin_44564.html</t>
   </si>
   <si>
-    <t>74HC00</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/kemet/C320C103K3G5TA/6656406</t>
   </si>
   <si>
@@ -1118,6 +1103,24 @@
   </si>
   <si>
     <t>1000uf Electroytic</t>
+  </si>
+  <si>
+    <t>* Note: This is an LS device and the clock may not operate correctly if an HC or other type of TTL device is used.</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/texas-instruments/SN74LS00N/277272</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/SN74LS00N/277272</t>
+  </si>
+  <si>
+    <t>* Note: This is an HC device and the clock may not operate correctly if an LS or other type of TTL device is used.</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/SN74LS00N?qs=spW5eSrOWB6G5wECF%252BEZFA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/SN74LS00N?qs=spW5eSrOWB6G5wECF%252BEZFA%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -2115,7 +2118,7 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2151,7 +2154,7 @@
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -2166,13 +2169,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -2189,7 +2192,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>74</v>
@@ -2206,7 +2209,7 @@
         <v>4016</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>75</v>
@@ -2223,7 +2226,7 @@
         <v>4023</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>76</v>
@@ -2243,7 +2246,7 @@
         <v>82</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>8</v>
@@ -2260,7 +2263,7 @@
         <v>4050</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>79</v>
@@ -2271,16 +2274,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>8</v>
@@ -2297,7 +2300,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>84</v>
@@ -2311,13 +2314,13 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>8</v>
@@ -2334,7 +2337,7 @@
         <v>4049</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>85</v>
@@ -2354,7 +2357,7 @@
         <v>83</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>8</v>
@@ -2371,10 +2374,13 @@
         <v>16</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>360</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>87</v>
+        <v>361</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -2388,10 +2394,13 @@
         <v>18</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>363</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2405,10 +2414,10 @@
         <v>4013</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -2416,7 +2425,7 @@
     </row>
     <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -2434,10 +2443,10 @@
         <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -2451,10 +2460,10 @@
         <v>32</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -2468,10 +2477,10 @@
         <v>34</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -2479,19 +2488,19 @@
         <v>1</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -2499,19 +2508,19 @@
         <v>1</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="E23" s="18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -2525,10 +2534,10 @@
         <v>3.58</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -2536,16 +2545,16 @@
         <v>1</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C25" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -2555,7 +2564,7 @@
     </row>
     <row r="27" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -2573,10 +2582,10 @@
         <v>39</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -2584,16 +2593,16 @@
         <v>1</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -2601,21 +2610,21 @@
         <v>2</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E30" s="14" t="s">
         <v>177</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -2627,16 +2636,16 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -2647,13 +2656,13 @@
         <v>22</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -2661,16 +2670,16 @@
         <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C35" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -2681,13 +2690,13 @@
         <v>23</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -2698,13 +2707,13 @@
         <v>24</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -2712,17 +2721,17 @@
         <v>1</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E38" s="12"/>
       <c r="F38" s="5" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -2733,13 +2742,13 @@
         <v>25</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -2750,13 +2759,13 @@
         <v>26</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F40" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -2767,18 +2776,18 @@
         <v>27</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -2792,10 +2801,10 @@
         <v>330</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -2809,10 +2818,10 @@
         <v>42</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -2826,10 +2835,10 @@
         <v>44</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -2843,10 +2852,10 @@
         <v>200</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -2860,10 +2869,10 @@
         <v>47</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -2871,16 +2880,16 @@
         <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -2888,19 +2897,19 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -2914,10 +2923,10 @@
         <v>42</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -2931,10 +2940,10 @@
         <v>52</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -2948,10 +2957,10 @@
         <v>52</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -2959,21 +2968,21 @@
         <v>2</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C54" s="1">
         <v>120</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -2994,7 +3003,7 @@
       </c>
       <c r="E57"/>
       <c r="F57" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -3012,7 +3021,7 @@
       </c>
       <c r="E58"/>
       <c r="F58" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -3030,7 +3039,7 @@
       </c>
       <c r="E59"/>
       <c r="F59" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -3048,7 +3057,7 @@
       </c>
       <c r="E60"/>
       <c r="F60" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -3056,16 +3065,16 @@
         <v>17</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="D61" t="s">
         <v>117</v>
       </c>
-      <c r="D61" t="s">
-        <v>118</v>
-      </c>
       <c r="E61" s="20" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F61" s="4"/>
     </row>
@@ -3080,11 +3089,11 @@
         <v>35</v>
       </c>
       <c r="D62" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E62"/>
       <c r="F62" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -3095,7 +3104,7 @@
     </row>
     <row r="64" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -3109,14 +3118,14 @@
         <v>37</v>
       </c>
       <c r="C65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D65" s="10" t="s">
         <v>121</v>
-      </c>
-      <c r="D65" s="10" t="s">
-        <v>122</v>
       </c>
       <c r="E65"/>
       <c r="F65" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -3130,10 +3139,10 @@
         <v>62</v>
       </c>
       <c r="D66" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F66" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -3147,11 +3156,11 @@
         <v>64</v>
       </c>
       <c r="D67" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E67"/>
       <c r="F67" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -3165,11 +3174,11 @@
         <v>63</v>
       </c>
       <c r="D68" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E68"/>
       <c r="F68" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -3177,16 +3186,16 @@
         <v>5</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D69" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="F69" s="5" t="s">
         <v>195</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -3194,16 +3203,16 @@
         <v>5</v>
       </c>
       <c r="B70" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>200</v>
-      </c>
       <c r="D70" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -3211,16 +3220,16 @@
         <v>4</v>
       </c>
       <c r="B71" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="D71" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F71" s="5" t="s">
         <v>180</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -3228,21 +3237,21 @@
         <v>5</v>
       </c>
       <c r="B72" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="C72" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="C72" s="17" t="s">
+      <c r="D72" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="F72" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
@@ -3254,18 +3263,18 @@
         <v>8</v>
       </c>
       <c r="B75" t="s">
+        <v>204</v>
+      </c>
+      <c r="D75" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="D75" s="6" t="s">
+      <c r="F75" s="5" t="s">
         <v>206</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
@@ -3277,10 +3286,10 @@
         <v>2</v>
       </c>
       <c r="B78" t="s">
+        <v>110</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -3294,7 +3303,7 @@
         <v>21</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -3357,7 +3366,7 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3391,7 +3400,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="21"/>
@@ -3407,13 +3416,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>8</v>
@@ -3430,11 +3439,11 @@
         <v>2</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -3448,11 +3457,11 @@
         <v>4016</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -3466,11 +3475,11 @@
         <v>4023</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -3487,7 +3496,7 @@
         <v>82</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>8</v>
@@ -3504,11 +3513,11 @@
         <v>4050</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -3516,16 +3525,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>80</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>8</v>
@@ -3542,11 +3551,11 @@
         <v>10</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -3557,13 +3566,13 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>8</v>
@@ -3580,11 +3589,11 @@
         <v>4049</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -3601,7 +3610,7 @@
         <v>83</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>8</v>
@@ -3618,11 +3627,13 @@
         <v>16</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14" s="12"/>
+        <v>95</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>360</v>
+      </c>
       <c r="F14" s="5" t="s">
-        <v>259</v>
+        <v>362</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -3636,11 +3647,13 @@
         <v>18</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E15" s="12"/>
+        <v>97</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>363</v>
+      </c>
       <c r="F15" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -3654,11 +3667,11 @@
         <v>4013</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -3671,7 +3684,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
@@ -3690,11 +3703,11 @@
         <v>30</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -3708,11 +3721,11 @@
         <v>32</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E20" s="12"/>
       <c r="F20" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -3726,11 +3739,11 @@
         <v>34</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -3738,19 +3751,19 @@
         <v>1</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>67</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -3758,19 +3771,19 @@
         <v>1</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C23" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>170</v>
-      </c>
       <c r="E23" s="26" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -3784,11 +3797,11 @@
         <v>3.58</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -3796,17 +3809,17 @@
         <v>1</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E25" s="12"/>
       <c r="F25" s="5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -3819,7 +3832,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B27" s="22"/>
       <c r="C27" s="21"/>
@@ -3838,11 +3851,11 @@
         <v>39</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -3850,16 +3863,16 @@
         <v>1</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>36</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F29" s="12"/>
     </row>
@@ -3868,16 +3881,16 @@
         <v>2</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D30" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="E30" s="26" t="s">
         <v>177</v>
-      </c>
-      <c r="E30" s="26" t="s">
-        <v>178</v>
       </c>
       <c r="F30" s="12"/>
     </row>
@@ -3891,7 +3904,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B32" s="22"/>
       <c r="C32" s="21"/>
@@ -3904,17 +3917,17 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -3925,14 +3938,14 @@
         <v>22</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -3940,17 +3953,17 @@
         <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C35" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -3961,14 +3974,14 @@
         <v>23</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -3979,14 +3992,14 @@
         <v>24</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E37" s="12"/>
       <c r="F37" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -3994,17 +4007,17 @@
         <v>1</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E38" s="12"/>
       <c r="F38" s="5" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -4015,14 +4028,14 @@
         <v>25</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E39" s="12"/>
       <c r="F39" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -4033,14 +4046,14 @@
         <v>26</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E40" s="12"/>
       <c r="F40" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -4051,14 +4064,14 @@
         <v>27</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E41" s="12"/>
       <c r="F41" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -4071,7 +4084,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B43" s="23"/>
       <c r="C43" s="12"/>
@@ -4090,11 +4103,11 @@
         <v>330</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E44" s="12"/>
       <c r="F44" s="5" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -4108,11 +4121,11 @@
         <v>42</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E45" s="12"/>
       <c r="F45" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -4126,11 +4139,11 @@
         <v>44</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E46" s="12"/>
       <c r="F46" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -4144,11 +4157,11 @@
         <v>200</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E47" s="12"/>
       <c r="F47" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -4162,11 +4175,11 @@
         <v>47</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E48" s="12"/>
       <c r="F48" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -4174,17 +4187,17 @@
         <v>3</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C49" s="12" t="s">
         <v>48</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E49" s="12"/>
       <c r="F49" s="4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -4192,19 +4205,19 @@
         <v>1</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C50" s="12" t="s">
         <v>49</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E50" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -4218,11 +4231,11 @@
         <v>42</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E51" s="12"/>
       <c r="F51" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -4236,11 +4249,11 @@
         <v>52</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E52" s="12"/>
       <c r="F52" s="4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -4254,11 +4267,11 @@
         <v>52</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E53" s="12"/>
       <c r="F53" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -4266,17 +4279,17 @@
         <v>2</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C54" s="12">
         <v>120</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E54" s="12"/>
       <c r="F54" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -4289,7 +4302,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B56" s="21"/>
       <c r="C56" s="21"/>
@@ -4312,7 +4325,7 @@
       </c>
       <c r="E57" s="23"/>
       <c r="F57" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -4330,7 +4343,7 @@
       </c>
       <c r="E58" s="23"/>
       <c r="F58" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -4348,7 +4361,7 @@
       </c>
       <c r="E59" s="23"/>
       <c r="F59" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -4366,7 +4379,7 @@
       </c>
       <c r="E60" s="23"/>
       <c r="F60" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -4374,16 +4387,16 @@
         <v>17</v>
       </c>
       <c r="B61" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C61" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C61" s="12" t="s">
+      <c r="D61" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="D61" s="23" t="s">
-        <v>118</v>
-      </c>
       <c r="E61" s="24" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F61" s="25"/>
     </row>
@@ -4398,11 +4411,11 @@
         <v>35</v>
       </c>
       <c r="D62" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E62" s="23"/>
       <c r="F62" s="4" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -4415,7 +4428,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B64" s="21"/>
       <c r="C64" s="21"/>
@@ -4431,14 +4444,14 @@
         <v>37</v>
       </c>
       <c r="C65" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D65" s="32" t="s">
         <v>121</v>
-      </c>
-      <c r="D65" s="32" t="s">
-        <v>122</v>
       </c>
       <c r="E65" s="23"/>
       <c r="F65" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -4452,11 +4465,11 @@
         <v>62</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E66" s="12"/>
       <c r="F66" s="4" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -4470,11 +4483,11 @@
         <v>64</v>
       </c>
       <c r="D67" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E67" s="23"/>
       <c r="F67" s="4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -4488,11 +4501,11 @@
         <v>63</v>
       </c>
       <c r="D68" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E68" s="23"/>
       <c r="F68" s="4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -4500,17 +4513,17 @@
         <v>5</v>
       </c>
       <c r="B69" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D69" s="33" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E69" s="12"/>
       <c r="F69" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -4518,17 +4531,17 @@
         <v>5</v>
       </c>
       <c r="B70" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="C70" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="C70" s="12" t="s">
-        <v>200</v>
-      </c>
       <c r="D70" s="33" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E70" s="12"/>
       <c r="F70" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -4536,17 +4549,17 @@
         <v>4</v>
       </c>
       <c r="B71" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="C71" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="C71" s="12" t="s">
-        <v>194</v>
-      </c>
       <c r="D71" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E71" s="12"/>
       <c r="F71" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -4554,17 +4567,17 @@
         <v>5</v>
       </c>
       <c r="B72" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="C72" s="33" t="s">
         <v>190</v>
       </c>
-      <c r="C72" s="33" t="s">
-        <v>191</v>
-      </c>
       <c r="D72" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E72" s="12"/>
       <c r="F72" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -4577,7 +4590,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B74" s="22"/>
       <c r="C74" s="21"/>
@@ -4590,15 +4603,15 @@
         <v>8</v>
       </c>
       <c r="B75" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C75" s="12"/>
       <c r="D75" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E75" s="12"/>
       <c r="F75" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -4611,7 +4624,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B77" s="22"/>
       <c r="C77" s="21"/>
@@ -4624,11 +4637,11 @@
         <v>2</v>
       </c>
       <c r="B78" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C78" s="12"/>
       <c r="D78" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E78" s="12"/>
       <c r="F78" s="12"/>
@@ -4644,7 +4657,7 @@
         <v>21</v>
       </c>
       <c r="D79" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E79" s="12"/>
       <c r="F79" s="12"/>
@@ -4713,8 +4726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC75F21-A609-2048-BDDD-710CC6135C01}">
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4750,7 +4763,7 @@
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -4765,13 +4778,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -4788,10 +4801,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -4805,10 +4818,10 @@
         <v>4016</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -4822,10 +4835,10 @@
         <v>4023</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -4842,7 +4855,7 @@
         <v>82</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>8</v>
@@ -4859,7 +4872,7 @@
         <v>4050</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>78</v>
@@ -4870,16 +4883,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>8</v>
@@ -4896,10 +4909,10 @@
         <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -4910,13 +4923,13 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>8</v>
@@ -4933,7 +4946,7 @@
         <v>4049</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>86</v>
@@ -4953,7 +4966,7 @@
         <v>83</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>8</v>
@@ -4967,13 +4980,16 @@
         <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>361</v>
+        <v>16</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>360</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>213</v>
+        <v>364</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -4987,10 +5003,13 @@
         <v>18</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>363</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -5004,15 +5023,15 @@
         <v>4013</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -5030,10 +5049,10 @@
         <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -5047,10 +5066,10 @@
         <v>32</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -5064,10 +5083,10 @@
         <v>34</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -5075,19 +5094,19 @@
         <v>1</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -5095,19 +5114,19 @@
         <v>1</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="E23" s="18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -5121,10 +5140,10 @@
         <v>3.58</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -5132,16 +5151,16 @@
         <v>1</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -5150,7 +5169,7 @@
     </row>
     <row r="27" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -5168,10 +5187,10 @@
         <v>39</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -5179,16 +5198,16 @@
         <v>1</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -5196,21 +5215,21 @@
         <v>2</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E30" s="14" t="s">
         <v>177</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -5222,16 +5241,16 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -5242,13 +5261,13 @@
         <v>22</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -5256,16 +5275,16 @@
         <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C35" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -5276,13 +5295,13 @@
         <v>23</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -5293,13 +5312,13 @@
         <v>24</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -5307,16 +5326,16 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -5327,13 +5346,13 @@
         <v>25</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -5344,13 +5363,13 @@
         <v>26</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -5361,18 +5380,18 @@
         <v>27</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -5386,10 +5405,10 @@
         <v>330</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -5403,10 +5422,10 @@
         <v>42</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -5420,10 +5439,10 @@
         <v>44</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -5437,10 +5456,10 @@
         <v>200</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -5454,10 +5473,10 @@
         <v>47</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -5465,16 +5484,16 @@
         <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -5482,19 +5501,19 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -5508,10 +5527,10 @@
         <v>42</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -5525,10 +5544,10 @@
         <v>52</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -5542,10 +5561,10 @@
         <v>52</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -5553,21 +5572,21 @@
         <v>2</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C54" s="1">
         <v>120</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -5587,7 +5606,7 @@
       </c>
       <c r="E57"/>
       <c r="F57" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -5605,7 +5624,7 @@
       </c>
       <c r="E58"/>
       <c r="F58" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -5623,7 +5642,7 @@
       </c>
       <c r="E59"/>
       <c r="F59" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -5647,16 +5666,16 @@
         <v>17</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="D61" t="s">
         <v>117</v>
       </c>
-      <c r="D61" t="s">
-        <v>118</v>
-      </c>
       <c r="E61" s="19" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F61"/>
     </row>
@@ -5671,11 +5690,11 @@
         <v>35</v>
       </c>
       <c r="D62" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E62"/>
       <c r="F62" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -5686,7 +5705,7 @@
     </row>
     <row r="64" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -5699,14 +5718,14 @@
         <v>37</v>
       </c>
       <c r="C65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D65" s="10" t="s">
         <v>121</v>
-      </c>
-      <c r="D65" s="10" t="s">
-        <v>122</v>
       </c>
       <c r="E65"/>
       <c r="F65" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -5720,10 +5739,10 @@
         <v>62</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -5737,11 +5756,11 @@
         <v>64</v>
       </c>
       <c r="D67" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E67"/>
       <c r="F67" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -5755,11 +5774,11 @@
         <v>63</v>
       </c>
       <c r="D68" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E68"/>
       <c r="F68" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5767,16 +5786,16 @@
         <v>5</v>
       </c>
       <c r="B69" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>200</v>
-      </c>
       <c r="D69" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -5784,16 +5803,16 @@
         <v>4</v>
       </c>
       <c r="B70" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="D70" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -5801,21 +5820,21 @@
         <v>5</v>
       </c>
       <c r="B71" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="C71" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="C71" s="17" t="s">
-        <v>191</v>
-      </c>
       <c r="D71" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="73" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
@@ -5827,18 +5846,18 @@
         <v>8</v>
       </c>
       <c r="B74" t="s">
+        <v>204</v>
+      </c>
+      <c r="D74" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="D74" s="6" t="s">
-        <v>206</v>
-      </c>
       <c r="F74" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="76" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
@@ -5850,10 +5869,10 @@
         <v>2</v>
       </c>
       <c r="B77" t="s">
+        <v>110</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -5867,7 +5886,7 @@
         <v>21</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -5929,8 +5948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9FDEFEA-849D-5B4C-9A76-0C1C74BD1400}">
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5966,7 +5985,7 @@
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -5981,13 +6000,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -6004,10 +6023,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -6021,10 +6040,10 @@
         <v>4016</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -6038,10 +6057,10 @@
         <v>4023</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -6058,7 +6077,7 @@
         <v>82</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>8</v>
@@ -6075,10 +6094,10 @@
         <v>4050</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -6086,16 +6105,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>8</v>
@@ -6112,10 +6131,10 @@
         <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -6126,13 +6145,13 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>8</v>
@@ -6149,10 +6168,10 @@
         <v>4049</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -6169,7 +6188,7 @@
         <v>83</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>8</v>
@@ -6186,10 +6205,13 @@
         <v>16</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>360</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>307</v>
+        <v>365</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -6203,10 +6225,13 @@
         <v>18</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>363</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -6220,15 +6245,15 @@
         <v>4013</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -6246,10 +6271,10 @@
         <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -6263,10 +6288,10 @@
         <v>32</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -6280,10 +6305,10 @@
         <v>34</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -6291,19 +6316,19 @@
         <v>1</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -6311,19 +6336,19 @@
         <v>1</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="E23" s="18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -6337,10 +6362,10 @@
         <v>3.58</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -6348,16 +6373,16 @@
         <v>1</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -6366,7 +6391,7 @@
     </row>
     <row r="27" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -6384,10 +6409,10 @@
         <v>39</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -6395,16 +6420,16 @@
         <v>1</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -6412,21 +6437,21 @@
         <v>2</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E30" s="14" t="s">
         <v>177</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -6438,16 +6463,16 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -6458,13 +6483,13 @@
         <v>22</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -6472,16 +6497,16 @@
         <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C35" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -6492,13 +6517,13 @@
         <v>23</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -6509,13 +6534,13 @@
         <v>24</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -6523,16 +6548,16 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D38" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>350</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -6543,13 +6568,13 @@
         <v>25</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -6560,13 +6585,13 @@
         <v>26</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -6577,18 +6602,18 @@
         <v>27</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -6602,10 +6627,10 @@
         <v>330</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -6619,10 +6644,10 @@
         <v>42</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -6636,10 +6661,10 @@
         <v>44</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -6653,10 +6678,10 @@
         <v>200</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -6670,10 +6695,10 @@
         <v>47</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -6681,16 +6706,16 @@
         <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -6698,19 +6723,19 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -6724,10 +6749,10 @@
         <v>42</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -6741,10 +6766,10 @@
         <v>52</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -6758,10 +6783,10 @@
         <v>52</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -6769,21 +6794,21 @@
         <v>2</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C54" s="1">
         <v>120</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -6803,7 +6828,7 @@
       </c>
       <c r="E57"/>
       <c r="F57" s="4" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -6821,7 +6846,7 @@
       </c>
       <c r="E58"/>
       <c r="F58" s="4" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -6839,7 +6864,7 @@
       </c>
       <c r="E59"/>
       <c r="F59" s="4" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -6863,16 +6888,16 @@
         <v>17</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="D61" t="s">
         <v>117</v>
       </c>
-      <c r="D61" t="s">
-        <v>118</v>
-      </c>
       <c r="E61" s="19" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F61"/>
     </row>
@@ -6887,11 +6912,11 @@
         <v>35</v>
       </c>
       <c r="D62" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E62"/>
       <c r="F62" s="4" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -6902,7 +6927,7 @@
     </row>
     <row r="64" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -6915,14 +6940,14 @@
         <v>37</v>
       </c>
       <c r="C65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D65" s="10" t="s">
         <v>121</v>
-      </c>
-      <c r="D65" s="10" t="s">
-        <v>122</v>
       </c>
       <c r="E65"/>
       <c r="F65" s="4" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -6936,10 +6961,10 @@
         <v>62</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -6953,11 +6978,11 @@
         <v>64</v>
       </c>
       <c r="D67" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E67"/>
       <c r="F67" s="4" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -6971,11 +6996,11 @@
         <v>63</v>
       </c>
       <c r="D68" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E68"/>
       <c r="F68" s="4" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -6983,16 +7008,16 @@
         <v>5</v>
       </c>
       <c r="B69" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>200</v>
-      </c>
       <c r="D69" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -7000,16 +7025,16 @@
         <v>4</v>
       </c>
       <c r="B70" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="D70" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7017,21 +7042,21 @@
         <v>5</v>
       </c>
       <c r="B71" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="C71" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="C71" s="17" t="s">
-        <v>191</v>
-      </c>
       <c r="D71" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="73" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
@@ -7043,18 +7068,18 @@
         <v>8</v>
       </c>
       <c r="B74" t="s">
+        <v>204</v>
+      </c>
+      <c r="D74" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="D74" s="6" t="s">
-        <v>206</v>
-      </c>
       <c r="F74" s="5" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="76" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
@@ -7066,10 +7091,10 @@
         <v>2</v>
       </c>
       <c r="B77" t="s">
+        <v>110</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -7083,7 +7108,7 @@
         <v>21</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix ELF II BOM per Randy Eubanks notes
</commit_message>
<xml_diff>
--- a/notes/ELF-II/AVI ELF II Final BOM.xlsx
+++ b/notes/ELF-II/AVI ELF II Final BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewwasson/Development/avi-elf-ii/notes/ELF-II/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC558B5-0ACA-9D44-9503-FE59DA7E70FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F693C7CC-8A97-6F4E-954F-A9DFC5FDC27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="600" windowWidth="42520" windowHeight="22300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27220" yWindow="2020" windowWidth="42520" windowHeight="22300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DigiKey.ca" sheetId="2" r:id="rId1"/>
@@ -5948,8 +5948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9FDEFEA-849D-5B4C-9A76-0C1C74BD1400}">
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6102,7 +6102,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>187</v>
@@ -6460,7 +6460,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
         <v>339</v>
@@ -6703,7 +6703,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B49" t="s">
         <v>208</v>
@@ -6720,7 +6720,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B50" t="s">
         <v>207</v>

</xml_diff>